<commit_message>
add struct to xlsx file and Constants
</commit_message>
<xml_diff>
--- a/fichier.xlsx
+++ b/fichier.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ababin/Documents/Dev/AppsInDev/Git/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ababin/Documents/Dev/AppsInDev/Git/ParseCoreXlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101B1D7B-36EB-7447-A616-DB6A1B11B10B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58335026-3693-1C41-BC1C-D667D581B591}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="21860" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pilotage des compétences" sheetId="5" r:id="rId1"/>
@@ -1119,7 +1119,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1127,7 +1127,7 @@
     <col min="1" max="1" width="30.6640625" customWidth="1"/>
     <col min="2" max="2" width="82" customWidth="1"/>
     <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="55.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="28">

</xml_diff>